<commit_message>
Revert "Performance Testing Data"
This reverts commit 760b7c200fcbd435cb19e4bbbca62e9ade508f22.
</commit_message>
<xml_diff>
--- a/Performance Data.xlsx
+++ b/Performance Data.xlsx
@@ -266,10 +266,8 @@
             <c:v>CPU Create Buffer</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -291,48 +289,78 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$13:$F$13</c:f>
+              <c:f>Sheet1!$B$3:$K$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.7</c:v>
+                  <c:v>0.78</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.63500000000000001</c:v>
+                  <c:v>0.62</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.62</c:v>
+                  <c:v>0.61</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.58000000000000007</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.58000000000000007</c:v>
+                  <c:v>0.61</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.53</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.63</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.51</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.65</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -346,10 +374,8 @@
             <c:v>CPU Write/Read</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
+            <a:ln w="19050" cap="rnd">
+              <a:noFill/>
               <a:round/>
             </a:ln>
             <a:effectLst/>
@@ -371,36 +397,51 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$14:$F$14</c:f>
+              <c:f>Sheet1!$B$4:$K$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.94499999999999995</c:v>
+                  <c:v>0.95</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.94</c:v>
@@ -409,10 +450,25 @@
                   <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.9</c:v>
+                  <c:v>0.94</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.90999999999999992</c:v>
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.89</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.84</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.98</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -426,7 +482,7 @@
             <c:v>CPU Set Arg</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -449,50 +505,108 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="0"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent3"/>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent3"/>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$15:$F$15</c:f>
+              <c:f>Sheet1!$B$5:$K$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.38500000000000001</c:v>
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.375</c:v>
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.38500000000000001</c:v>
+                  <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.38500000000000001</c:v>
+                  <c:v>0.37</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.38</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -506,7 +620,7 @@
             <c:v>CPU Run Kernel</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="25400" cap="rnd">
+            <a:ln w="19050" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -531,48 +645,78 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$16:$F$16</c:f>
+              <c:f>Sheet1!$B$6:$K$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.75</c:v>
+                  <c:v>1.73</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1.77</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1.81</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>2.1</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>4.2350000000000003</c:v>
+                  <c:v>1.81</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>30.68</c:v>
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.06</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.75</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.72</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>30.16</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>31.2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -588,7 +732,7 @@
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent2"/>
               </a:solidFill>
               <a:round/>
             </a:ln>
@@ -611,48 +755,78 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$18:$F$18</c:f>
+              <c:f>Sheet1!$B$8:$K$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.6100000000000001</c:v>
+                  <c:v>0.54</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.68</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.66</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.67999999999999994</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.63500000000000001</c:v>
+                  <c:v>0.66</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.66500000000000004</c:v>
+                  <c:v>0.67</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.69</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.57999999999999996</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.66</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -691,47 +865,77 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$19:$F$19</c:f>
+              <c:f>Sheet1!$B$9:$K$9</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.86499999999999999</c:v>
+                  <c:v>0.79</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.94</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.86</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>0.96</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.89</c:v>
-                </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="5">
+                  <c:v>0.96</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.93</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.85</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.91</c:v>
+                </c:pt>
+                <c:pt idx="9">
                   <c:v>0.91</c:v>
                 </c:pt>
               </c:numCache>
@@ -775,48 +979,78 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$20:$F$20</c:f>
+              <c:f>Sheet1!$B$10:$K$10</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>0.39500000000000002</c:v>
+                  <c:v>0.38</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>0.39</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.42499999999999999</c:v>
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>0.39</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.46</c:v>
+                  <c:v>0.41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.44</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.39</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.54</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.38</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -857,50 +1091,112 @@
               <a:effectLst/>
             </c:spPr>
           </c:marker>
+          <c:dPt>
+            <c:idx val="6"/>
+            <c:marker>
+              <c:symbol val="circle"/>
+              <c:size val="5"/>
+              <c:spPr>
+                <a:solidFill>
+                  <a:schemeClr val="accent2">
+                    <a:lumMod val="60000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:ln w="9525">
+                  <a:solidFill>
+                    <a:schemeClr val="accent2">
+                      <a:lumMod val="60000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+            </c:marker>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:ln w="25400" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:dPt>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$12:$F$12</c:f>
+              <c:f>Sheet1!$B$2:$K$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>100</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
+                  <c:v>100</c:v>
+                </c:pt>
+                <c:pt idx="4">
                   <c:v>1000</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="5">
+                  <c:v>1000</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>10000</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>1000000</c:v>
+                <c:pt idx="7">
+                  <c:v>10000</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>100000</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>100000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$21:$F$21</c:f>
+              <c:f>Sheet1!$B$11:$K$11</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="5"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
-                  <c:v>1.655</c:v>
+                  <c:v>1.61</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>1.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>1.64</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>1.83</c:v>
-                </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.3</c:v>
+                  <c:v>1.64</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>29.734999999999999</c:v>
+                  <c:v>1.8</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.86</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.31</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.29</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>29.83</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>29.64</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -915,79 +1211,33 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1893478288"/>
-        <c:axId val="1893474480"/>
+        <c:axId val="568043360"/>
+        <c:axId val="572251056"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="1893478288"/>
+        <c:axId val="568043360"/>
         <c:scaling>
           <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Faces in Initial Mesh</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
+        <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1023,12 +1273,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1893474480"/>
+        <c:crossAx val="572251056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="1893474480"/>
+        <c:axId val="572251056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1048,83 +1298,8 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:minorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="5000"/>
-                  <a:lumOff val="95000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:minorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Runtime</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> (ms)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1160,7 +1335,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1893478288"/>
+        <c:crossAx val="568043360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1173,7 +1348,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1278,11 +1453,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Stream</a:t>
+              <a:t>CubicVR Processing vs.</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Compaction vs. Sequential Remove</a:t>
+              <a:t> Fracture Time</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1321,159 +1496,117 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="stacked"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Parallel</c:v>
+            <c:v>Fracture Time</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$24:$E$24</c:f>
+              <c:f>Sheet1!$B$25:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>712</c:v>
+                  <c:v>32000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2176</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4528</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$25:$E$25</c:f>
+              <c:f>Sheet1!$B$26:$D$26</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>1785.5</c:v>
+                  <c:v>1054</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5081.5</c:v>
+                  <c:v>2307</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>7817</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>11210</c:v>
+                  <c:v>3757</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Sequential</c:v>
+            <c:v>CubicVR Add to Scene</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$24:$E$24</c:f>
+              <c:f>Sheet1!$B$25:$D$25</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>7000</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>712</c:v>
+                  <c:v>32000</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2176</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>4528</c:v>
+                  <c:v>40000</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$26:$E$26</c:f>
+              <c:f>Sheet1!$B$27:$D$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>184</c:v>
+                  <c:v>164</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>712.5</c:v>
+                  <c:v>236</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>1180</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>1942</c:v>
+                  <c:v>785</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="r"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -1481,80 +1614,20 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1848426800"/>
-        <c:axId val="1848432784"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1848426800"/>
+        <c:gapWidth val="150"/>
+        <c:overlap val="100"/>
+        <c:axId val="664618720"/>
+        <c:axId val="664616544"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="664618720"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number of Triangles</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> on Initial Mesh</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
@@ -1562,8 +1635,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -1590,17 +1663,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848432784"/>
+        <c:crossAx val="664616544"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="1848432784"/>
+        <c:axId val="664616544"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -1615,76 +1691,14 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Runtime (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
+        <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -1708,9 +1722,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848426800"/>
+        <c:crossAx val="664618720"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -1721,7 +1735,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -1824,7 +1838,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CPU vs GPU Fracture Time</a:t>
+              <a:t>Parallel</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> vs. Sequential Intersection</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1862,103 +1880,168 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="clustered"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>GPU</c:v>
+            <c:v>Parallel</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$28:$C$28</c:f>
+              <c:f>Sheet1!$B$20:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8415</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7937</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>854</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$29:$C$29</c:f>
+              <c:f>Sheet1!$B$21:$F$21</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>713.7</c:v>
+                  <c:v>339</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>532.54999999999995</c:v>
+                  <c:v>305</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>318</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>328</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>289</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>CPU</c:v>
+            <c:v>Sequential</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$28:$C$28</c:f>
+              <c:f>Sheet1!$B$20:$F$20</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>8415</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>7937</c:v>
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>308</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>324</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>854</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$30:$C$30</c:f>
+              <c:f>Sheet1!$B$22:$F$22</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="2"/>
+                <c:ptCount val="5"/>
                 <c:pt idx="0">
-                  <c:v>700.5</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>541.9</c:v>
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>64</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>222</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -1968,82 +2051,31 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="182"/>
-        <c:axId val="1848431152"/>
-        <c:axId val="1848429520"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1848431152"/>
+        <c:axId val="660176704"/>
+        <c:axId val="665283008"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="660176704"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number of Triangles</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>on Initial Mesh</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2053,8 +2085,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2081,20 +2113,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848429520"/>
+        <c:crossAx val="665283008"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1848429520"/>
+        <c:axId val="665283008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2109,70 +2138,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Runtime (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2196,9 +2175,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848431152"/>
+        <c:crossAx val="660176704"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2312,11 +2291,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>CubicVR Processing vs.</a:t>
+              <a:t>Stream</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Fracture Time</a:t>
+              <a:t> Compaction vs. Sequential Remove</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -2355,115 +2334,180 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:barChart>
-        <c:barDir val="bar"/>
-        <c:grouping val="stacked"/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Fracture Time</c:v>
+            <c:v>Parallel</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$38:$D$38</c:f>
+              <c:f>Sheet1!$B$13:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7000</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32000</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40000</c:v>
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2176</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$39:$D$39</c:f>
+              <c:f>Sheet1!$B$14:$G$14</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>1054</c:v>
+                  <c:v>1888</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2307</c:v>
+                  <c:v>1683</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>3757</c:v>
+                  <c:v>4162</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7817</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11210</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>CubicVR Add to Scene</c:v>
+            <c:v>Sequential</c:v>
           </c:tx>
           <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent2"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$B$38:$D$38</c:f>
+              <c:f>Sheet1!$B$13:$G$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>7000</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>32000</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>40000</c:v>
+                  <c:v>730</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>684</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2176</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>4528</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:cat>
-          <c:val>
+          </c:xVal>
+          <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$40:$D$40</c:f>
+              <c:f>Sheet1!$B$15:$G$15</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="3"/>
+                <c:ptCount val="6"/>
                 <c:pt idx="0">
-                  <c:v>164</c:v>
+                  <c:v>189</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>236</c:v>
+                  <c:v>179</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>785</c:v>
+                  <c:v>430</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>995</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1180</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1942</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:val>
+          </c:yVal>
+          <c:smooth val="1"/>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -2473,88 +2517,31 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:overlap val="100"/>
-        <c:axId val="1893469584"/>
-        <c:axId val="1893471760"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="1893469584"/>
+        <c:axId val="659031680"/>
+        <c:axId val="660178880"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="659031680"/>
         <c:scaling>
+          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number of </a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>Triangles</a:t>
-                </a:r>
-              </a:p>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr/>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t>on Initial Mesh</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
           <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+        </c:majorGridlines>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -2564,8 +2551,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -2592,20 +2579,17 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1893471760"/>
+        <c:crossAx val="660178880"/>
         <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
       <c:valAx>
-        <c:axId val="1893471760"/>
+        <c:axId val="660178880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
+        <c:axPos val="l"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -2620,70 +2604,20 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Runtime (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln>
-            <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -2707,9 +2641,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1893469584"/>
+        <c:crossAx val="659031680"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
+        <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -2823,11 +2757,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Parallel</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t> vs. Sequential Intersection</a:t>
+              <a:t>CPU vs GPU Fracture Time</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -2865,282 +2795,103 @@
     <c:autoTitleDeleted val="0"/>
     <c:plotArea>
       <c:layout/>
-      <c:scatterChart>
-        <c:scatterStyle val="smoothMarker"/>
+      <c:barChart>
+        <c:barDir val="bar"/>
+        <c:grouping val="clustered"/>
         <c:varyColors val="0"/>
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Parallel</c:v>
+            <c:v>GPU</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent1"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$31:$E$31</c:f>
+              <c:f>Sheet1!$B$17:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>8415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>308</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>854</c:v>
+                  <c:v>7937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$32:$E$32</c:f>
+              <c:f>Sheet1!$B$18:$C$18</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>322</c:v>
+                  <c:v>713.7</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>323</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>289</c:v>
+                  <c:v>532.54999999999995</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
         </c:ser>
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Sequential</c:v>
+            <c:v>CPU</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
             </a:ln>
             <a:effectLst/>
           </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:dLbls>
-            <c:dLbl>
-              <c:idx val="3"/>
-              <c:dLblPos val="r"/>
-              <c:showLegendKey val="0"/>
-              <c:showVal val="1"/>
-              <c:showCatName val="1"/>
-              <c:showSerName val="0"/>
-              <c:showPercent val="0"/>
-              <c:showBubbleSize val="0"/>
-              <c:extLst>
-                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}"/>
-              </c:extLst>
-            </c:dLbl>
-            <c:spPr>
-              <a:noFill/>
-              <a:ln>
-                <a:noFill/>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-            <c:txPr>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
-                <a:spAutoFit/>
-              </a:bodyPr>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="75000"/>
-                        <a:lumOff val="25000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:endParaRPr lang="en-US"/>
-              </a:p>
-            </c:txPr>
-            <c:showLegendKey val="0"/>
-            <c:showVal val="0"/>
-            <c:showCatName val="0"/>
-            <c:showSerName val="0"/>
-            <c:showPercent val="0"/>
-            <c:showBubbleSize val="0"/>
-            <c:extLst>
-              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
-                <c15:showLeaderLines val="1"/>
-                <c15:leaderLines>
-                  <c:spPr>
-                    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-                      <a:solidFill>
-                        <a:schemeClr val="tx1">
-                          <a:lumMod val="35000"/>
-                          <a:lumOff val="65000"/>
-                        </a:schemeClr>
-                      </a:solidFill>
-                      <a:round/>
-                    </a:ln>
-                    <a:effectLst/>
-                  </c:spPr>
-                </c15:leaderLines>
-              </c:ext>
-            </c:extLst>
-          </c:dLbls>
-          <c:xVal>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$B$31:$E$31</c:f>
+              <c:f>Sheet1!$B$17:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>12</c:v>
+                  <c:v>8415</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>308</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>854</c:v>
+                  <c:v>7937</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:xVal>
-          <c:yVal>
+          </c:cat>
+          <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$33:$E$33</c:f>
+              <c:f>Sheet1!$B$19:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="2"/>
                 <c:pt idx="0">
-                  <c:v>25</c:v>
+                  <c:v>700.5</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>97.5</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>222</c:v>
+                  <c:v>541.9</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
-          </c:yVal>
-          <c:smooth val="1"/>
+          </c:val>
         </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
@@ -3150,77 +2901,17 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="1848430064"/>
-        <c:axId val="1848421360"/>
-      </c:scatterChart>
-      <c:valAx>
-        <c:axId val="1848430064"/>
+        <c:gapWidth val="182"/>
+        <c:axId val="659033856"/>
+        <c:axId val="659034944"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="659033856"/>
         <c:scaling>
-          <c:logBase val="10"/>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Number</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-US" baseline="0"/>
-                  <a:t> of Triangles on Initial Mesh</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
+        <c:axPos val="l"/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -3230,8 +2921,8 @@
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
               <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -3258,17 +2949,20 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848421360"/>
+        <c:crossAx val="659034944"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
-      </c:valAx>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
       <c:valAx>
-        <c:axId val="1848421360"/>
+        <c:axId val="659034944"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
-        <c:axPos val="l"/>
+        <c:axPos val="b"/>
         <c:majorGridlines>
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
@@ -3283,76 +2977,14 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-US"/>
-                  <a:t>Runtime (ms)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:layout/>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-US"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:spPr>
           <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
+          <a:ln>
+            <a:noFill/>
           </a:ln>
           <a:effectLst/>
         </c:spPr>
@@ -3376,9 +3008,9 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1848430064"/>
+        <c:crossAx val="659033856"/>
         <c:crosses val="autoZero"/>
-        <c:crossBetween val="midCat"/>
+        <c:crossBetween val="between"/>
       </c:valAx>
       <c:spPr>
         <a:noFill/>
@@ -3389,7 +3021,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -4174,7 +3806,7 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4201,8 +3833,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4303,7 +3935,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4335,10 +3967,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -4659,17 +4291,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -4690,7 +4311,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -4717,8 +4338,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -4819,7 +4440,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -4851,10 +4472,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -5175,6 +4796,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -5195,7 +4827,7 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="297">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5222,8 +4854,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5324,7 +4956,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="28575" cap="rnd">
+      <a:ln w="19050" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -5356,10 +4988,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -5680,6 +5312,17 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -5700,7 +5343,7 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="216">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5727,8 +5370,8 @@
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
           <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -5829,7 +5472,7 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:ln w="19050" cap="rnd">
+      <a:ln w="28575" cap="rnd">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
         </a:solidFill>
@@ -5861,10 +5504,10 @@
     <cs:lnRef idx="0">
       <cs:styleClr val="auto"/>
     </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="rnd">
@@ -6185,17 +5828,6 @@
         <a:lumOff val="35000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:valueAxis>
   <cs:wall>
@@ -6219,16 +5851,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>190501</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>23</xdr:row>
-      <xdr:rowOff>390525</xdr:rowOff>
+      <xdr:col>27</xdr:col>
+      <xdr:colOff>238125</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6249,20 +5881,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>229719</xdr:colOff>
-      <xdr:row>5</xdr:row>
-      <xdr:rowOff>78441</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>330572</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>6722</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>571500</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>145675</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>179293</xdr:colOff>
+      <xdr:row>74</xdr:row>
+      <xdr:rowOff>67235</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="5" name="Chart 4"/>
+        <xdr:cNvPr id="3" name="Chart 2"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6279,20 +5911,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>252131</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>246529</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>532279</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>163606</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>11206</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>26894</xdr:rowOff>
+      <xdr:col>31</xdr:col>
+      <xdr:colOff>44823</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>168088</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvPr id="4" name="Chart 3"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6309,20 +5941,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>352983</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>67237</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>453837</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>29135</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>33</xdr:col>
-      <xdr:colOff>11205</xdr:colOff>
-      <xdr:row>42</xdr:row>
-      <xdr:rowOff>179296</xdr:rowOff>
+      <xdr:col>30</xdr:col>
+      <xdr:colOff>582705</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>56029</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2"/>
+        <xdr:cNvPr id="5" name="Chart 4"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6339,20 +5971,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>386602</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>156882</xdr:rowOff>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>498662</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>224118</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>593911</xdr:colOff>
-      <xdr:row>64</xdr:row>
-      <xdr:rowOff>89647</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>56029</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>105334</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvPr id="6" name="Chart 5"/>
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
@@ -6633,10 +6265,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K40"/>
+  <dimension ref="A1:K27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D26" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="AC24" sqref="AC24"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C19" sqref="B18:C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6992,47 +6624,38 @@
     </row>
     <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
-      <c r="B12" s="3">
-        <v>10</v>
-      </c>
-      <c r="C12" s="3">
-        <v>100</v>
-      </c>
-      <c r="D12" s="3">
-        <v>1000</v>
-      </c>
-      <c r="E12" s="3">
-        <v>10000</v>
-      </c>
-      <c r="F12" s="3">
-        <v>1000000</v>
-      </c>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
+      <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
       <c r="J12" s="3"/>
       <c r="K12" s="3"/>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B13">
-        <f>AVERAGE(B3:C3)</f>
-        <v>0.7</v>
-      </c>
-      <c r="C13">
-        <f>AVERAGE(D3:E3)</f>
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="D13">
-        <f>AVERAGE(F3:G3)</f>
-        <v>0.62</v>
-      </c>
-      <c r="E13">
-        <f>AVERAGE(H3:I3)</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="F13">
-        <f>AVERAGE(J3:K3)</f>
-        <v>0.58000000000000007</v>
+    <row r="13" spans="1:11" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="4">
+        <v>12</v>
+      </c>
+      <c r="C13" s="4">
+        <v>12</v>
+      </c>
+      <c r="D13" s="4">
+        <v>730</v>
+      </c>
+      <c r="E13" s="4">
+        <v>684</v>
+      </c>
+      <c r="F13" s="4">
+        <v>2176</v>
+      </c>
+      <c r="G13" s="4">
+        <v>4528</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -7040,51 +6663,53 @@
       <c r="K13" s="3"/>
     </row>
     <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14">
-        <f t="shared" ref="B14:B21" si="0">AVERAGE(B4:C4)</f>
-        <v>0.94499999999999995</v>
-      </c>
-      <c r="C14">
-        <f t="shared" ref="C14:C21" si="1">AVERAGE(D4:E4)</f>
-        <v>0.94</v>
-      </c>
-      <c r="D14">
-        <f t="shared" ref="D14:D21" si="2">AVERAGE(F4:G4)</f>
-        <v>0.94</v>
-      </c>
-      <c r="E14">
-        <f t="shared" ref="E14:E21" si="3">AVERAGE(H4:I4)</f>
-        <v>0.9</v>
-      </c>
-      <c r="F14">
-        <f t="shared" ref="F14:F21" si="4">AVERAGE(J4:K4)</f>
-        <v>0.90999999999999992</v>
+      <c r="A14" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" s="4">
+        <v>1888</v>
+      </c>
+      <c r="C14" s="4">
+        <v>1683</v>
+      </c>
+      <c r="D14" s="4">
+        <v>4162</v>
+      </c>
+      <c r="E14" s="4">
+        <v>6001</v>
+      </c>
+      <c r="F14" s="4">
+        <v>7817</v>
+      </c>
+      <c r="G14" s="4">
+        <v>11210</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
       <c r="J14" s="3"/>
       <c r="K14" s="3"/>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15">
-        <f t="shared" si="0"/>
-        <v>0.38</v>
-      </c>
-      <c r="C15">
-        <f t="shared" si="1"/>
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="D15">
-        <f t="shared" si="2"/>
-        <v>0.375</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="3"/>
-        <v>0.38500000000000001</v>
-      </c>
-      <c r="F15">
-        <f t="shared" si="4"/>
-        <v>0.38500000000000001</v>
+    <row r="15" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="4">
+        <v>189</v>
+      </c>
+      <c r="C15" s="4">
+        <v>179</v>
+      </c>
+      <c r="D15" s="4">
+        <v>430</v>
+      </c>
+      <c r="E15" s="4">
+        <v>995</v>
+      </c>
+      <c r="F15" s="4">
+        <v>1180</v>
+      </c>
+      <c r="G15" s="4">
+        <v>1942</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -7092,399 +6717,246 @@
       <c r="K15" s="3"/>
     </row>
     <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16">
-        <f t="shared" si="0"/>
-        <v>1.75</v>
-      </c>
-      <c r="C16">
-        <f t="shared" si="1"/>
-        <v>1.81</v>
-      </c>
-      <c r="D16">
-        <f t="shared" si="2"/>
-        <v>2.1</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="3"/>
-        <v>4.2350000000000003</v>
-      </c>
-      <c r="F16">
-        <f t="shared" si="4"/>
-        <v>30.68</v>
-      </c>
+      <c r="A16" s="1"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
+      <c r="G16" s="3"/>
       <c r="H16" s="3"/>
       <c r="I16" s="3"/>
       <c r="J16" s="3"/>
       <c r="K16" s="3"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B18">
-        <f t="shared" si="0"/>
-        <v>0.6100000000000001</v>
-      </c>
-      <c r="C18">
-        <f t="shared" si="1"/>
-        <v>0.66</v>
-      </c>
-      <c r="D18">
-        <f t="shared" si="2"/>
-        <v>0.67999999999999994</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
-        <v>0.63500000000000001</v>
-      </c>
-      <c r="F18">
-        <f t="shared" si="4"/>
-        <v>0.66500000000000004</v>
-      </c>
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B17" s="4">
+        <v>8415</v>
+      </c>
+      <c r="C17" s="4">
+        <v>7937</v>
+      </c>
+      <c r="D17" s="4">
+        <v>8069</v>
+      </c>
+      <c r="E17" s="4">
+        <v>8553</v>
+      </c>
+      <c r="F17" s="3"/>
+      <c r="G17" s="3"/>
+      <c r="H17" s="3"/>
+      <c r="I17" s="3"/>
+      <c r="J17" s="3"/>
+      <c r="K17" s="3"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="B19">
-        <f t="shared" si="0"/>
-        <v>0.86499999999999999</v>
-      </c>
-      <c r="C19">
-        <f t="shared" si="1"/>
-        <v>0.86</v>
-      </c>
-      <c r="D19">
-        <f t="shared" si="2"/>
-        <v>0.96</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="3"/>
-        <v>0.89</v>
-      </c>
-      <c r="F19">
-        <f t="shared" si="4"/>
-        <v>0.91</v>
-      </c>
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="4">
+        <v>713.7</v>
+      </c>
+      <c r="C18" s="4">
+        <v>532.54999999999995</v>
+      </c>
+      <c r="F18" s="3"/>
+      <c r="G18" s="3"/>
+      <c r="H18" s="3"/>
+      <c r="I18" s="3"/>
+      <c r="J18" s="3"/>
+      <c r="K18" s="3"/>
+    </row>
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19" s="4">
+        <v>700.5</v>
+      </c>
+      <c r="C19" s="4">
+        <v>541.9</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
+      <c r="G19" s="3"/>
+      <c r="H19" s="3"/>
+      <c r="I19" s="3"/>
+      <c r="J19" s="3"/>
+      <c r="K19" s="3"/>
     </row>
     <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20">
-        <f t="shared" si="0"/>
-        <v>0.39500000000000002</v>
-      </c>
-      <c r="C20">
-        <f t="shared" si="1"/>
-        <v>0.39</v>
-      </c>
-      <c r="D20">
-        <f t="shared" si="2"/>
-        <v>0.42499999999999999</v>
-      </c>
-      <c r="E20">
-        <f t="shared" si="3"/>
-        <v>0.39</v>
-      </c>
-      <c r="F20">
-        <f t="shared" si="4"/>
-        <v>0.46</v>
-      </c>
+      <c r="A20" s="1"/>
+      <c r="B20" s="4">
+        <v>12</v>
+      </c>
+      <c r="C20" s="4">
+        <v>12</v>
+      </c>
+      <c r="D20" s="4">
+        <v>308</v>
+      </c>
+      <c r="E20" s="4">
+        <v>324</v>
+      </c>
+      <c r="F20" s="4">
+        <v>854</v>
+      </c>
+      <c r="G20" s="1"/>
+      <c r="H20" s="3"/>
+      <c r="I20" s="3"/>
+      <c r="J20" s="3"/>
+      <c r="K20" s="3"/>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21">
-        <f t="shared" si="0"/>
-        <v>1.655</v>
-      </c>
-      <c r="C21">
-        <f t="shared" si="1"/>
-        <v>1.64</v>
-      </c>
-      <c r="D21">
-        <f t="shared" si="2"/>
-        <v>1.83</v>
-      </c>
-      <c r="E21">
-        <f t="shared" si="3"/>
-        <v>3.3</v>
-      </c>
-      <c r="F21">
-        <f t="shared" si="4"/>
-        <v>29.734999999999999</v>
+    <row r="21" spans="1:11" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B21" s="4">
+        <v>339</v>
+      </c>
+      <c r="C21" s="4">
+        <v>305</v>
+      </c>
+      <c r="D21" s="4">
+        <v>318</v>
+      </c>
+      <c r="E21" s="4">
+        <v>328</v>
+      </c>
+      <c r="F21" s="4">
+        <v>289</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="H21" s="3"/>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
       <c r="K21" s="3"/>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="4">
+        <v>39</v>
+      </c>
+      <c r="C22" s="4">
+        <v>11</v>
+      </c>
+      <c r="D22" s="4">
+        <v>64</v>
+      </c>
+      <c r="E22" s="4">
+        <v>131</v>
+      </c>
+      <c r="F22" s="4">
+        <v>222</v>
+      </c>
+      <c r="G22" s="3"/>
       <c r="H22" s="3"/>
       <c r="I22" s="3"/>
       <c r="J22" s="3"/>
       <c r="K22" s="3"/>
     </row>
     <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="H23" s="3"/>
-      <c r="I23" s="3"/>
+      <c r="A23" s="1"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="1"/>
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+      <c r="I23" s="1"/>
       <c r="J23" s="3"/>
       <c r="K23" s="3"/>
     </row>
-    <row r="24" spans="1:11" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="B24" s="4">
         <v>12</v>
       </c>
       <c r="C24" s="4">
-        <v>712</v>
+        <v>12</v>
       </c>
       <c r="D24" s="4">
-        <v>2176</v>
-      </c>
-      <c r="E24" s="4">
-        <v>4528</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+      <c r="G24" s="3"/>
       <c r="H24" s="3"/>
       <c r="I24" s="3"/>
       <c r="J24" s="3"/>
       <c r="K24" s="3"/>
     </row>
     <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="1" t="s">
-        <v>11</v>
-      </c>
+      <c r="A25" s="1"/>
       <c r="B25" s="4">
-        <v>1785.5</v>
+        <v>7000</v>
       </c>
       <c r="C25" s="4">
-        <v>5081.5</v>
+        <v>32000</v>
       </c>
       <c r="D25" s="4">
-        <v>7817</v>
-      </c>
-      <c r="E25" s="4">
-        <v>11210</v>
-      </c>
-      <c r="H25" s="3"/>
-      <c r="I25" s="3"/>
+        <v>40000</v>
+      </c>
+      <c r="E25" s="1"/>
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+      <c r="I25" s="1"/>
       <c r="J25" s="3"/>
       <c r="K25" s="3"/>
     </row>
     <row r="26" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="1" t="s">
-        <v>10</v>
+        <v>17</v>
       </c>
       <c r="B26" s="4">
-        <v>184</v>
+        <v>1054</v>
       </c>
       <c r="C26" s="4">
-        <v>712.5</v>
+        <v>2307</v>
       </c>
       <c r="D26" s="4">
-        <v>1180</v>
-      </c>
-      <c r="E26" s="4">
-        <v>1942</v>
-      </c>
+        <v>3757</v>
+      </c>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+      <c r="G26" s="3"/>
       <c r="H26" s="3"/>
       <c r="I26" s="3"/>
       <c r="J26" s="3"/>
       <c r="K26" s="3"/>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="1"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="3"/>
+    <row r="27" spans="1:11" ht="27" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B27" s="4">
+        <v>164</v>
+      </c>
+      <c r="C27" s="4">
+        <v>236</v>
+      </c>
+      <c r="D27" s="4">
+        <v>785</v>
+      </c>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
       <c r="G27" s="3"/>
-      <c r="H27" s="1"/>
-      <c r="I27" s="1"/>
+      <c r="H27" s="3"/>
+      <c r="I27" s="3"/>
       <c r="J27" s="3"/>
       <c r="K27" s="3"/>
-    </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="4">
-        <v>8415</v>
-      </c>
-      <c r="C28" s="4">
-        <v>7937</v>
-      </c>
-      <c r="D28" s="4">
-        <v>8069</v>
-      </c>
-      <c r="E28" s="4">
-        <v>8553</v>
-      </c>
-      <c r="F28" s="3"/>
-      <c r="G28" s="3"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-    </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B29" s="4">
-        <v>713.7</v>
-      </c>
-      <c r="C29" s="4">
-        <v>532.54999999999995</v>
-      </c>
-      <c r="F29" s="3"/>
-      <c r="G29" s="3"/>
-      <c r="H29" s="1"/>
-      <c r="I29" s="1"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-    </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B30" s="4">
-        <v>700.5</v>
-      </c>
-      <c r="C30" s="4">
-        <v>541.9</v>
-      </c>
-      <c r="D30" s="3"/>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="3"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3"/>
-    </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="1"/>
-      <c r="B31" s="4">
-        <v>12</v>
-      </c>
-      <c r="C31" s="4">
-        <v>308</v>
-      </c>
-      <c r="D31" s="4">
-        <v>854</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="G31" s="1"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3"/>
-    </row>
-    <row r="32" spans="1:11" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B32" s="4">
-        <v>322</v>
-      </c>
-      <c r="C32" s="4">
-        <v>323</v>
-      </c>
-      <c r="D32" s="4">
-        <v>289</v>
-      </c>
-      <c r="E32" s="4"/>
-      <c r="G32" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="52.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B33" s="4">
-        <v>25</v>
-      </c>
-      <c r="C33" s="4">
-        <v>97.5</v>
-      </c>
-      <c r="D33" s="4">
-        <v>222</v>
-      </c>
-      <c r="E33" s="4"/>
-      <c r="G33" s="3"/>
-    </row>
-    <row r="34" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A34" s="1"/>
-      <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="1"/>
-      <c r="F34" s="1"/>
-      <c r="G34" s="1"/>
-    </row>
-    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
-      <c r="G35" s="3"/>
-    </row>
-    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E36" s="1"/>
-      <c r="F36" s="1"/>
-      <c r="G36" s="1"/>
-    </row>
-    <row r="37" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B37" s="4">
-        <v>12</v>
-      </c>
-      <c r="C37" s="4">
-        <v>12</v>
-      </c>
-      <c r="D37" s="4">
-        <v>12</v>
-      </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="1"/>
-      <c r="B38" s="4">
-        <v>7000</v>
-      </c>
-      <c r="C38" s="4">
-        <v>32000</v>
-      </c>
-      <c r="D38" s="4">
-        <v>40000</v>
-      </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="3"/>
-    </row>
-    <row r="39" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="4">
-        <v>1054</v>
-      </c>
-      <c r="C39" s="4">
-        <v>2307</v>
-      </c>
-      <c r="D39" s="4">
-        <v>3757</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B40" s="4">
-        <v>164</v>
-      </c>
-      <c r="C40" s="4">
-        <v>236</v>
-      </c>
-      <c r="D40" s="4">
-        <v>785</v>
-      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>